<commit_message>
Cleaned up the code.
</commit_message>
<xml_diff>
--- a/commonData.xlsx
+++ b/commonData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Item</t>
   </si>
@@ -94,6 +94,27 @@
   </si>
   <si>
     <t>annual FD Increase</t>
+  </si>
+  <si>
+    <t>http://economictimes.indiatimes.com/news/economy/policy/number-of-registered-companies-climbs-to-15-27-lakh-in-january/articleshow/51026331.cms</t>
+  </si>
+  <si>
+    <t>Registered Companies</t>
+  </si>
+  <si>
+    <t>companies</t>
+  </si>
+  <si>
+    <t>Active Companies</t>
+  </si>
+  <si>
+    <t>petty cash Min</t>
+  </si>
+  <si>
+    <t>http://www.quickbooks.in/r/accounting-taxes/creating-a-petty-cash-system/</t>
+  </si>
+  <si>
+    <t>petty cash Max</t>
   </si>
 </sst>
 </file>
@@ -426,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -642,6 +663,65 @@
         <v>1000000000</v>
       </c>
       <c r="D14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>15.27</v>
+      </c>
+      <c r="C15" s="1">
+        <v>100000</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16">
+        <v>10.76</v>
+      </c>
+      <c r="C16" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>6000</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>30000</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>